<commit_message>
Improve data source parsing and dashboard visuals
</commit_message>
<xml_diff>
--- a/data/planilha_referencia.xlsx
+++ b/data/planilha_referencia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillherme\Desktop\Alura\projeto_macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillherme\Desktop\Alura\projeto_macro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C1916A-5553-424F-8CC9-9407EFD825C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5859BF32-4F5F-4E5D-A015-03FBD499A55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20235" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Ouro Futuros</t>
   </si>
@@ -59,12 +59,6 @@
     <t>The Global Dow USD</t>
   </si>
   <si>
-    <t>Vale SA ADR</t>
-  </si>
-  <si>
-    <t>Petroleo Brasileiro Petrobras SA ADR</t>
-  </si>
-  <si>
     <t>iShares MSCI Brazil ETF</t>
   </si>
   <si>
@@ -230,13 +224,7 @@
     <t>Ativo</t>
   </si>
   <si>
-    <t>https://www.marketwatch.com/investing/stock/pbr</t>
-  </si>
-  <si>
-    <t>https://www.marketwatch.com/investing/stock/vale</t>
-  </si>
-  <si>
-    <t>https://www.marketwatch.com/investing/currency/usdkrw</t>
+    <t>https://br.investing.com/indices/f-usdkrw</t>
   </si>
 </sst>
 </file>
@@ -599,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,374 +601,352 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B30" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>1</v>
+      <c r="A31" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B31" s="5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="4">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C33" t="s">
-        <v>59</v>
+      <c r="C31" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1" xr:uid="{04C25C18-C1D3-4942-8955-1CFED8444ADC}"/>
-    <hyperlink ref="C30" r:id="rId2" xr:uid="{DDB268F8-2704-48F3-9C42-F72DCA337B37}"/>
-    <hyperlink ref="C29" r:id="rId3" xr:uid="{03BD0C16-B23C-4D21-BE59-3C0EBE6E595C}"/>
-    <hyperlink ref="C27" r:id="rId4" xr:uid="{5098B5F2-CB02-4E9E-A3C5-1C0F082F0660}"/>
-    <hyperlink ref="C28" r:id="rId5" xr:uid="{4AE043E8-6D76-483E-9978-4E6B3FED9A8C}"/>
+    <hyperlink ref="C30" r:id="rId1" xr:uid="{04C25C18-C1D3-4942-8955-1CFED8444ADC}"/>
+    <hyperlink ref="C28" r:id="rId2" xr:uid="{DDB268F8-2704-48F3-9C42-F72DCA337B37}"/>
+    <hyperlink ref="C27" r:id="rId3" xr:uid="{03BD0C16-B23C-4D21-BE59-3C0EBE6E595C}"/>
+    <hyperlink ref="C25" r:id="rId4" xr:uid="{5098B5F2-CB02-4E9E-A3C5-1C0F082F0660}"/>
+    <hyperlink ref="C26" r:id="rId5" xr:uid="{4AE043E8-6D76-483E-9978-4E6B3FED9A8C}"/>
     <hyperlink ref="C23" r:id="rId6" xr:uid="{81F274C7-9241-4061-9F70-86569BB4922E}"/>
     <hyperlink ref="C22" r:id="rId7" xr:uid="{97020A93-59E8-456A-83BC-AE7C45F28864}"/>
     <hyperlink ref="C21" r:id="rId8" xr:uid="{FDF483FA-BC52-4EEA-B508-D04CD3C74880}"/>
@@ -1002,8 +968,7 @@
     <hyperlink ref="C5" r:id="rId24" xr:uid="{3F6C79E4-773A-4576-8B9B-8E17D5EA302A}"/>
     <hyperlink ref="C3" r:id="rId25" xr:uid="{EB9F093A-A9F9-4F96-89AE-9A14FA4FD221}"/>
     <hyperlink ref="C2" r:id="rId26" xr:uid="{7AD11042-A619-4858-8938-BADF5FA95C8B}"/>
-    <hyperlink ref="C31" r:id="rId27" xr:uid="{EBEA042A-6F35-4273-86DF-FD7793144527}"/>
-    <hyperlink ref="C25" r:id="rId28" xr:uid="{FE9FEBFC-1D56-4272-A850-FC256D36B5A4}"/>
+    <hyperlink ref="C29" r:id="rId27" xr:uid="{EBEA042A-6F35-4273-86DF-FD7793144527}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>